<commit_message>
Updated for this year
</commit_message>
<xml_diff>
--- a/Labs/Lab4/Assignment4Rubric.xlsx
+++ b/Labs/Lab4/Assignment4Rubric.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Repos\CS246-CourseMaterials\Labs\Lab4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4A1C45-0CCA-4A1D-8E34-9B1F29D0DCE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECAE127-148C-6C49-9AFD-BD7A276084A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="495" windowWidth="10620" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="14760" yWindow="500" windowWidth="13920" windowHeight="14640" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Requirements</t>
   </si>
@@ -43,47 +43,47 @@
     <t>CS246 Assignment 5 Rubric</t>
   </si>
   <si>
-    <t>Software Proposal for a Real Client</t>
-  </si>
-  <si>
-    <t>5A Proposal</t>
-  </si>
-  <si>
-    <t>5B Contract</t>
-  </si>
-  <si>
-    <t>Cover letter</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Project overview</t>
-  </si>
-  <si>
-    <t>Estimate</t>
-  </si>
-  <si>
-    <t>Deployment &amp; Documentation</t>
-  </si>
-  <si>
-    <t>Cost and terms</t>
-  </si>
-  <si>
-    <t>Timeframe &amp; workflow</t>
-  </si>
-  <si>
     <t>CS246 Assignment 4 Rubric</t>
   </si>
   <si>
     <t>OO Design with UML</t>
+  </si>
+  <si>
+    <t>Prose description of a game</t>
+  </si>
+  <si>
+    <t>List of nouns and verbs</t>
+  </si>
+  <si>
+    <t>Games: Craps, Pig, or Ship, Captain, Crew (or student choice)</t>
+  </si>
+  <si>
+    <t>UI not included in this design</t>
+  </si>
+  <si>
+    <t>UML class diagram</t>
+  </si>
+  <si>
+    <t>List of classes, props, fields, methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Classes with props, fields, methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Relationships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Cardinality (multiplicity)</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,10 +127,18 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,6 +169,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,144 +487,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="B7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="5" customFormat="1">
       <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="5" customFormat="1">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <f>SUM(B6:B12)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="5" customFormat="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <f>SUM(B6:B11)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2">
-        <f>SUM(B15:B17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B6:B17)</f>
-        <v>100</v>
-      </c>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -622,183 +630,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
         <v>20</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="5" customFormat="1">
       <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2">
-        <f>SUM(B6:B11)</f>
-        <v>50</v>
-      </c>
-      <c r="C12" s="2">
-        <f>SUM(C6:C11)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="B13" s="2">
+        <f>SUM(B6:B12)</f>
+        <v>100</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C6:C12)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2">
-        <f>SUM(B15:B17)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <f>SUM(C15:C17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B6:B17)</f>
-        <v>100</v>
-      </c>
-      <c r="C20" s="2">
-        <f>SUM(C6:C17)</f>
-        <v>100</v>
-      </c>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added week 6 overview
</commit_message>
<xml_diff>
--- a/Labs/Lab4/Assignment4Rubric.xlsx
+++ b/Labs/Lab4/Assignment4Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935A4E49-07AA-A24E-B3B6-EFAB18C3C6C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CEFCF-422E-7348-95A5-5F695A9920CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="500" windowWidth="13920" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="9960" yWindow="600" windowWidth="13920" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Requirements</t>
   </si>
@@ -80,6 +91,18 @@
   </si>
   <si>
     <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Good choices</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Correctly done</t>
   </si>
 </sst>
 </file>
@@ -164,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,13 +202,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -206,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,7 +669,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -658,7 +678,7 @@
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="1.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -674,22 +694,22 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
@@ -705,7 +725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="17">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -715,9 +735,11 @@
       <c r="C6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -727,9 +749,11 @@
       <c r="C7" s="2">
         <v>15</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -739,7 +763,9 @@
       <c r="C8" s="2">
         <v>20</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
@@ -749,7 +775,7 @@
       <c r="C9" s="2"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="17">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -759,9 +785,11 @@
       <c r="C10" s="2">
         <v>15</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -771,9 +799,11 @@
       <c r="C11" s="2">
         <v>20</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1">
+      <c r="E11" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="17">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -783,7 +813,9 @@
       <c r="C12" s="2">
         <v>15</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
@@ -839,5 +871,6 @@
     <mergeCell ref="A4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>